<commit_message>
Hasta la vista, Baby! TUCUTUCUTUCUTUCU
</commit_message>
<xml_diff>
--- a/análisis/Diccionario de Datos v2.xlsx
+++ b/análisis/Diccionario de Datos v2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="72">
   <si>
     <t>Continente</t>
   </si>
@@ -82,7 +82,10 @@
     <t>imagen</t>
   </si>
   <si>
-    <t>Nombre de la imagen representativa del continente</t>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Nombre de la imagen representativa del continente generado de forma única y aleatoria, tiene un tamaño de 18 porque el algoritmo para crear un id único crea un string de 13 letras, sumándole 1 carácter por el punto de la extensión y 4 por la extensión en siNombre de la imagen representativa del continente</t>
   </si>
   <si>
     <t>Situacion</t>
@@ -112,10 +115,7 @@
     <t>Texto profundizando y dando información sobre la situación</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>Nombre de la imagen de la situación</t>
+    <t>Nombre de la imagen de la situación generado de forma única y aleatoria, tiene un tamaño de 18 porque el algoritmo para crear un id único crea un string de 13 letras, sumándole 1 carácter por el punto de la extensión y 4 por la extensión en si</t>
   </si>
   <si>
     <t>Conflicto</t>
@@ -136,13 +136,19 @@
     <t xml:space="preserve">tinyint </t>
   </si>
   <si>
+    <t>default NULL</t>
+  </si>
+  <si>
     <t>Número del motivo correcto</t>
   </si>
   <si>
-    <t>datosInicio</t>
-  </si>
-  <si>
-    <t>Texto en el que se proporcionan datos sobre la fecha en la que inició del conflicto</t>
+    <t>fechaInicio</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Fecha en la que inició del conflicto</t>
   </si>
   <si>
     <t>Motivo</t>
@@ -227,7 +233,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -251,6 +257,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -283,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -304,9 +314,15 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -607,7 +623,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="4">
-        <v>255.0</v>
+        <v>2000.0</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>10</v>
@@ -643,18 +659,18 @@
         <v>15</v>
       </c>
       <c r="C8" s="4">
-        <v>15.0</v>
+        <v>18.0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="4" t="s">
         <v>23</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -682,10 +698,10 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>10</v>
@@ -696,8 +712,8 @@
       <c r="F12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>27</v>
+      <c r="G12" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13">
@@ -712,16 +728,16 @@
         <v>10</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>18</v>
@@ -733,7 +749,7 @@
         <v>10</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
@@ -744,7 +760,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="5">
-        <v>255.0</v>
+        <v>2000.0</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>10</v>
@@ -752,7 +768,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16">
@@ -763,12 +779,12 @@
         <v>15</v>
       </c>
       <c r="C16" s="4">
-        <v>15.0</v>
+        <v>18.0</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -805,7 +821,7 @@
         <v>36</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>10</v>
@@ -813,7 +829,7 @@
       <c r="E20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -826,25 +842,24 @@
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="G21" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="4">
-        <v>255.0</v>
+        <v>44</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>10</v>
@@ -852,12 +867,12 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26">
@@ -888,7 +903,7 @@
         <v>36</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>10</v>
@@ -896,7 +911,7 @@
       <c r="E27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -916,18 +931,18 @@
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="4">
-        <v>255.0</v>
+        <v>2000.0</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>10</v>
@@ -935,12 +950,12 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32">
@@ -968,10 +983,10 @@
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>10</v>
@@ -979,19 +994,19 @@
       <c r="E33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>50</v>
+      <c r="G33" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="5">
-        <v>255.0</v>
+      <c r="C34" s="9">
+        <v>2000.0</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>10</v>
@@ -999,12 +1014,12 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37">
@@ -1032,10 +1047,10 @@
     </row>
     <row r="38">
       <c r="A38" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>10</v>
@@ -1043,13 +1058,13 @@
       <c r="E38" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G38" s="7" t="s">
-        <v>50</v>
+      <c r="G38" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>40</v>
@@ -1063,18 +1078,18 @@
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C40" s="4">
-        <v>255.0</v>
+        <v>2000.0</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>10</v>
@@ -1082,15 +1097,15 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="5" t="s">
@@ -1099,12 +1114,12 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44">
@@ -1132,10 +1147,10 @@
     </row>
     <row r="45">
       <c r="A45" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>10</v>
@@ -1143,19 +1158,19 @@
       <c r="E45" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F45" s="8" t="s">
+      <c r="F45" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G45" s="7" t="s">
-        <v>64</v>
+      <c r="G45" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="5" t="s">
@@ -1164,12 +1179,12 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>15</v>
@@ -1181,7 +1196,7 @@
         <v>10</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>